<commit_message>
Checked the values in the manual calculations file with a fine tooth and comb.
Green = good to go
</commit_message>
<xml_diff>
--- a/graphics_scripts/data/manual_calculations.xlsx
+++ b/graphics_scripts/data/manual_calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5660" windowHeight="5460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="30">
   <si>
     <t>data set</t>
   </si>
@@ -87,13 +87,40 @@
   </si>
   <si>
     <t>Tsalikian2005</t>
+  </si>
+  <si>
+    <t>1636-69-35</t>
+  </si>
+  <si>
+    <t>subject 43</t>
+  </si>
+  <si>
+    <t>subject 15</t>
+  </si>
+  <si>
+    <t>subject 11</t>
+  </si>
+  <si>
+    <t>subject 8</t>
+  </si>
+  <si>
+    <t>subject 44</t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>microscopic gap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +128,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -134,13 +181,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,1453 +474,1491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="8.7265625" style="2"/>
+    <col min="4" max="4" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="J1" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5">
         <v>59</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>52</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>60</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>352</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>118</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>353</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>645</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="6">
         <v>264</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>646</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>939</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="6">
         <v>183</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>940</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>1233</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="6">
         <v>150</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
         <v>244</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="11">
         <v>31</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>245</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>531</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="6">
         <v>107</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>532</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>754</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="6">
         <v>83</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>755</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>849</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="6">
         <v>91</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>1</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>849</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>1101</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="6">
         <v>58</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="8">
         <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>1102</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>1379</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="6">
         <v>51</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>1380</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>1666</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="6">
         <v>57</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>1667</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>1846</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="6">
         <v>34</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="8">
         <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="J14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>1847</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>2124</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="6">
         <v>53</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>2125</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>2303</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="6">
         <v>65</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="G16" s="5">
+        <v>1</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>2304</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>2585</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="6">
         <v>47</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="8">
         <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="J17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>7697</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>7953</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="4">
         <v>52</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="5">
         <v>1</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>7954</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>8128</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="4">
         <v>75</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>8129</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>8343</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="4">
         <v>46</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>1</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>8344</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>8513</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="4">
         <v>40</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>1</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>8514</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>8745</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="4">
         <v>61</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>405</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>644</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="6">
         <v>47</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="5">
         <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="5">
         <v>2</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>2994</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>3281</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="6">
         <v>70</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+      <c r="H24" s="5">
         <v>2</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="5">
         <v>3282</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>3569</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="6">
         <v>81</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="5">
         <v>2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="5">
         <v>3570</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>3857</v>
       </c>
       <c r="D26" s="2">
         <v>154</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="5">
         <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
+      <c r="H26" s="5">
         <v>2</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="5">
         <v>3858</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="5">
         <v>4144</v>
       </c>
       <c r="D27" s="2">
-        <v>71</v>
-      </c>
-      <c r="E27">
+        <v>104</v>
+      </c>
+      <c r="E27" s="5">
         <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
         <v>2</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <v>4145</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <v>4432</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="6">
         <v>95</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>0</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
+      <c r="G28" s="5">
+        <v>1</v>
+      </c>
+      <c r="H28" s="5">
         <v>2</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="5">
         <v>5746</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="5">
         <v>5842</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="6">
         <v>89</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="8">
         <v>0</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
         <v>2</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="J29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>7413</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="5">
         <v>7698</v>
       </c>
       <c r="D30" s="2">
-        <v>67</v>
-      </c>
-      <c r="E30">
+        <v>75</v>
+      </c>
+      <c r="E30" s="5">
         <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
         <v>2</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>7699</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="5">
         <v>7985</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="6">
         <v>58</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="5">
         <v>0</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
         <v>2</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="5">
         <v>7986</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="5">
         <v>8273</v>
       </c>
       <c r="D32" s="2">
-        <v>50</v>
-      </c>
-      <c r="E32">
+        <v>45</v>
+      </c>
+      <c r="E32" s="5">
         <v>0</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-      <c r="H32">
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
         <v>2</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="5">
         <v>8274</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>8561</v>
       </c>
       <c r="D33" s="2">
-        <v>41</v>
-      </c>
-      <c r="E33">
+        <v>69</v>
+      </c>
+      <c r="E33" s="5">
         <v>0</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
+      <c r="G33" s="5">
+        <v>1</v>
+      </c>
+      <c r="H33" s="5">
         <v>2</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="5">
         <v>8562</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>8849</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="6">
         <v>32</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="5">
         <v>0</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
+      <c r="G34" s="5">
+        <v>1</v>
+      </c>
+      <c r="H34" s="5">
         <v>2</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="5">
         <v>11018</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>11301</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="6">
         <v>120</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="8">
         <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
+      <c r="G35" s="5">
+        <v>1</v>
+      </c>
+      <c r="H35" s="5">
         <v>2</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="J35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="5">
         <v>11302</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="5">
         <v>11588</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="6">
         <v>211</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="5">
         <v>0</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-      <c r="H36">
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+      <c r="H36" s="5">
         <v>2</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="5">
         <v>11589</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="5">
         <v>11830</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="6">
         <v>147</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="5">
         <v>1</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="H37">
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
         <v>2</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="5">
         <v>11831</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="5">
         <v>12118</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="6">
         <v>125</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="5">
         <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="G38">
-        <v>1</v>
-      </c>
-      <c r="H38">
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
         <v>2</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="5">
         <v>12119</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="5">
         <v>12406</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="6">
         <v>227</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="5">
         <v>0</v>
       </c>
       <c r="F39">
         <v>0</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
         <v>2</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="5">
         <v>12653</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="5">
         <v>12940</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="6">
         <v>153</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="5">
         <v>0</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
         <v>2</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5">
         <v>135</v>
       </c>
-      <c r="D41" s="2">
-        <v>144</v>
-      </c>
-      <c r="E41">
+      <c r="D41" s="6">
+        <v>138</v>
+      </c>
+      <c r="E41" s="5">
         <v>0</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>1</v>
+      </c>
+      <c r="I41" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="5">
         <v>136</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="5">
         <v>242</v>
       </c>
-      <c r="D42" s="2">
-        <v>96</v>
-      </c>
-      <c r="E42">
+      <c r="D42" s="4">
+        <v>164</v>
+      </c>
+      <c r="E42" s="5">
         <v>0</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1</v>
+      </c>
+      <c r="I42" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="5">
         <v>243</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="5">
         <v>384</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="6">
         <v>135</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="5">
         <v>0</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>1</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>385</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>455</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="4">
         <v>15</v>
       </c>
-      <c r="E44" s="4">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4">
-        <v>1</v>
-      </c>
-      <c r="G44" s="4">
-        <v>0</v>
-      </c>
-      <c r="H44" s="4">
-        <v>1</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>1</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="5">
         <v>456</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="5">
         <v>561</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="6">
         <v>45</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="5">
         <v>0</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="5">
         <v>1601</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="5">
         <v>1755</v>
       </c>
-      <c r="D46" s="2">
-        <v>69</v>
-      </c>
-      <c r="E46">
+      <c r="D46" s="6">
+        <v>55</v>
+      </c>
+      <c r="E46" s="5">
         <v>0</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+      <c r="H46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="5">
         <v>3076</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="5">
         <v>3230</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="6">
         <v>87</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="5">
         <v>0</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="G47" s="5">
+        <v>0</v>
+      </c>
+      <c r="H47" s="5">
+        <v>1</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="5">
         <v>3319</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="5">
         <v>3475</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="6">
         <v>360</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="5">
         <v>0</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="G48" s="5">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="5">
         <v>3549</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="5">
         <v>3701</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="6">
         <v>105</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="5">
         <v>0</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="G49" s="5">
+        <v>0</v>
+      </c>
+      <c r="H49" s="5">
+        <v>1</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="5">
         <v>4272</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="5">
         <v>4423</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="6">
         <v>283</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="5">
         <v>0</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
+      <c r="G50" s="5">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2 new manual calculations to Dubosson and modified the load_data script
</commit_message>
<xml_diff>
--- a/graphics_scripts/data/manual_calculations.xlsx
+++ b/graphics_scripts/data/manual_calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
   <si>
     <t>data set</t>
   </si>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,7 +649,7 @@
       <c r="E6" s="5">
         <v>0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>0</v>
       </c>
       <c r="G6" s="5">
@@ -664,60 +664,58 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5">
-        <v>1</v>
+        <v>1497</v>
       </c>
       <c r="C7" s="5">
-        <v>244</v>
-      </c>
-      <c r="D7" s="11">
-        <v>31</v>
+        <v>1787</v>
+      </c>
+      <c r="D7" s="6">
+        <v>266</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>0</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
       </c>
       <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
-        <v>245</v>
+        <v>1788</v>
       </c>
       <c r="C8" s="5">
-        <v>531</v>
+        <v>2078</v>
       </c>
       <c r="D8" s="6">
-        <v>107</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8">
+        <v>166</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
         <v>0</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -725,13 +723,13 @@
         <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>532</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>754</v>
-      </c>
-      <c r="D9" s="6">
-        <v>83</v>
+        <v>244</v>
+      </c>
+      <c r="D9" s="11">
+        <v>31</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -754,16 +752,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="5">
-        <v>755</v>
+        <v>245</v>
       </c>
       <c r="C10" s="5">
-        <v>849</v>
+        <v>531</v>
       </c>
       <c r="D10" s="6">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="E10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -783,15 +781,15 @@
         <v>10</v>
       </c>
       <c r="B11" s="5">
-        <v>849</v>
+        <v>532</v>
       </c>
       <c r="C11" s="5">
-        <v>1101</v>
+        <v>754</v>
       </c>
       <c r="D11" s="6">
-        <v>58</v>
-      </c>
-      <c r="E11" s="8">
+        <v>83</v>
+      </c>
+      <c r="E11" s="5">
         <v>0</v>
       </c>
       <c r="F11">
@@ -805,9 +803,6 @@
       </c>
       <c r="I11" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -815,16 +810,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <v>1102</v>
+        <v>755</v>
       </c>
       <c r="C12" s="5">
-        <v>1379</v>
+        <v>849</v>
       </c>
       <c r="D12" s="6">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -836,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -844,15 +839,15 @@
         <v>10</v>
       </c>
       <c r="B13" s="5">
-        <v>1380</v>
+        <v>849</v>
       </c>
       <c r="C13" s="5">
-        <v>1666</v>
+        <v>1101</v>
       </c>
       <c r="D13" s="6">
-        <v>57</v>
-      </c>
-      <c r="E13" s="5">
+        <v>58</v>
+      </c>
+      <c r="E13" s="8">
         <v>0</v>
       </c>
       <c r="F13">
@@ -865,7 +860,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -873,15 +871,15 @@
         <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>1667</v>
+        <v>1102</v>
       </c>
       <c r="C14" s="5">
-        <v>1846</v>
+        <v>1379</v>
       </c>
       <c r="D14" s="6">
-        <v>34</v>
-      </c>
-      <c r="E14" s="8">
+        <v>51</v>
+      </c>
+      <c r="E14" s="5">
         <v>0</v>
       </c>
       <c r="F14">
@@ -895,9 +893,6 @@
       </c>
       <c r="I14" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="J14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -905,13 +900,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="5">
-        <v>1847</v>
+        <v>1380</v>
       </c>
       <c r="C15" s="5">
-        <v>2124</v>
+        <v>1666</v>
       </c>
       <c r="D15" s="6">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -934,16 +929,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="5">
-        <v>2125</v>
+        <v>1667</v>
       </c>
       <c r="C16" s="5">
-        <v>2303</v>
+        <v>1846</v>
       </c>
       <c r="D16" s="6">
-        <v>65</v>
-      </c>
-      <c r="E16" s="5">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -956,6 +951,9 @@
       </c>
       <c r="I16" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -963,15 +961,15 @@
         <v>10</v>
       </c>
       <c r="B17" s="5">
-        <v>2304</v>
+        <v>1847</v>
       </c>
       <c r="C17" s="5">
-        <v>2585</v>
+        <v>2124</v>
       </c>
       <c r="D17" s="6">
-        <v>47</v>
-      </c>
-      <c r="E17" s="8">
+        <v>53</v>
+      </c>
+      <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17">
@@ -985,9 +983,6 @@
       </c>
       <c r="I17" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="J17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -995,13 +990,13 @@
         <v>10</v>
       </c>
       <c r="B18" s="5">
-        <v>7697</v>
+        <v>2125</v>
       </c>
       <c r="C18" s="5">
-        <v>7953</v>
-      </c>
-      <c r="D18" s="4">
-        <v>52</v>
+        <v>2303</v>
+      </c>
+      <c r="D18" s="6">
+        <v>65</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1016,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -1024,16 +1019,16 @@
         <v>10</v>
       </c>
       <c r="B19" s="5">
-        <v>7954</v>
+        <v>2304</v>
       </c>
       <c r="C19" s="5">
-        <v>8128</v>
-      </c>
-      <c r="D19" s="4">
-        <v>75</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
+        <v>2585</v>
+      </c>
+      <c r="D19" s="6">
+        <v>47</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1045,7 +1040,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -1053,13 +1051,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="5">
-        <v>8129</v>
+        <v>7697</v>
       </c>
       <c r="C20" s="5">
-        <v>8343</v>
+        <v>7953</v>
       </c>
       <c r="D20" s="4">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1082,13 +1080,13 @@
         <v>10</v>
       </c>
       <c r="B21" s="5">
-        <v>8344</v>
+        <v>7954</v>
       </c>
       <c r="C21" s="5">
-        <v>8513</v>
+        <v>8128</v>
       </c>
       <c r="D21" s="4">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1111,13 +1109,13 @@
         <v>10</v>
       </c>
       <c r="B22" s="5">
-        <v>8514</v>
+        <v>8129</v>
       </c>
       <c r="C22" s="5">
-        <v>8745</v>
+        <v>8343</v>
       </c>
       <c r="D22" s="4">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -1137,16 +1135,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B23" s="5">
-        <v>405</v>
+        <v>8344</v>
       </c>
       <c r="C23" s="5">
-        <v>644</v>
-      </c>
-      <c r="D23" s="6">
-        <v>47</v>
+        <v>8513</v>
+      </c>
+      <c r="D23" s="4">
+        <v>40</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -1158,27 +1156,27 @@
         <v>1</v>
       </c>
       <c r="H23" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B24" s="5">
-        <v>2994</v>
+        <v>8514</v>
       </c>
       <c r="C24" s="5">
-        <v>3281</v>
-      </c>
-      <c r="D24" s="6">
-        <v>70</v>
+        <v>8745</v>
+      </c>
+      <c r="D24" s="4">
+        <v>61</v>
       </c>
       <c r="E24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1187,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="H24" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -1198,16 +1196,16 @@
         <v>13</v>
       </c>
       <c r="B25" s="5">
-        <v>3282</v>
+        <v>405</v>
       </c>
       <c r="C25" s="5">
-        <v>3569</v>
+        <v>644</v>
       </c>
       <c r="D25" s="6">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="E25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1219,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -1227,13 +1225,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="5">
-        <v>3570</v>
+        <v>2994</v>
       </c>
       <c r="C26" s="5">
-        <v>3857</v>
-      </c>
-      <c r="D26" s="2">
-        <v>154</v>
+        <v>3281</v>
+      </c>
+      <c r="D26" s="6">
+        <v>70</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
@@ -1256,13 +1254,13 @@
         <v>13</v>
       </c>
       <c r="B27" s="5">
-        <v>3858</v>
+        <v>3282</v>
       </c>
       <c r="C27" s="5">
-        <v>4144</v>
-      </c>
-      <c r="D27" s="2">
-        <v>104</v>
+        <v>3569</v>
+      </c>
+      <c r="D27" s="6">
+        <v>81</v>
       </c>
       <c r="E27" s="5">
         <v>0</v>
@@ -1285,13 +1283,13 @@
         <v>13</v>
       </c>
       <c r="B28" s="5">
-        <v>4145</v>
+        <v>3570</v>
       </c>
       <c r="C28" s="5">
-        <v>4432</v>
-      </c>
-      <c r="D28" s="6">
-        <v>95</v>
+        <v>3857</v>
+      </c>
+      <c r="D28" s="2">
+        <v>154</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
@@ -1314,19 +1312,19 @@
         <v>13</v>
       </c>
       <c r="B29" s="5">
-        <v>5746</v>
+        <v>3858</v>
       </c>
       <c r="C29" s="5">
-        <v>5842</v>
-      </c>
-      <c r="D29" s="6">
-        <v>89</v>
-      </c>
-      <c r="E29" s="8">
+        <v>4144</v>
+      </c>
+      <c r="D29" s="2">
+        <v>104</v>
+      </c>
+      <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="5">
         <v>1</v>
@@ -1335,10 +1333,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -1346,13 +1341,13 @@
         <v>13</v>
       </c>
       <c r="B30" s="5">
-        <v>7413</v>
+        <v>4145</v>
       </c>
       <c r="C30" s="5">
-        <v>7698</v>
-      </c>
-      <c r="D30" s="2">
-        <v>75</v>
+        <v>4432</v>
+      </c>
+      <c r="D30" s="6">
+        <v>95</v>
       </c>
       <c r="E30" s="5">
         <v>0</v>
@@ -1367,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -1375,19 +1370,19 @@
         <v>13</v>
       </c>
       <c r="B31" s="5">
-        <v>7699</v>
+        <v>5746</v>
       </c>
       <c r="C31" s="5">
-        <v>7985</v>
+        <v>5842</v>
       </c>
       <c r="D31" s="6">
-        <v>58</v>
-      </c>
-      <c r="E31" s="5">
+        <v>89</v>
+      </c>
+      <c r="E31" s="8">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="5">
         <v>1</v>
@@ -1396,7 +1391,10 @@
         <v>2</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="J31" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -1404,13 +1402,13 @@
         <v>13</v>
       </c>
       <c r="B32" s="5">
-        <v>7986</v>
+        <v>7413</v>
       </c>
       <c r="C32" s="5">
-        <v>8273</v>
+        <v>7698</v>
       </c>
       <c r="D32" s="2">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="E32" s="5">
         <v>0</v>
@@ -1433,13 +1431,13 @@
         <v>13</v>
       </c>
       <c r="B33" s="5">
-        <v>8274</v>
+        <v>7699</v>
       </c>
       <c r="C33" s="5">
-        <v>8561</v>
-      </c>
-      <c r="D33" s="2">
-        <v>69</v>
+        <v>7985</v>
+      </c>
+      <c r="D33" s="6">
+        <v>58</v>
       </c>
       <c r="E33" s="5">
         <v>0</v>
@@ -1462,13 +1460,13 @@
         <v>13</v>
       </c>
       <c r="B34" s="5">
-        <v>8562</v>
+        <v>7986</v>
       </c>
       <c r="C34" s="5">
-        <v>8849</v>
-      </c>
-      <c r="D34" s="6">
-        <v>32</v>
+        <v>8273</v>
+      </c>
+      <c r="D34" s="2">
+        <v>45</v>
       </c>
       <c r="E34" s="5">
         <v>0</v>
@@ -1491,15 +1489,15 @@
         <v>13</v>
       </c>
       <c r="B35" s="5">
-        <v>11018</v>
+        <v>8274</v>
       </c>
       <c r="C35" s="5">
-        <v>11301</v>
-      </c>
-      <c r="D35" s="6">
-        <v>120</v>
-      </c>
-      <c r="E35" s="8">
+        <v>8561</v>
+      </c>
+      <c r="D35" s="2">
+        <v>69</v>
+      </c>
+      <c r="E35" s="5">
         <v>0</v>
       </c>
       <c r="F35">
@@ -1512,10 +1510,7 @@
         <v>2</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -1523,13 +1518,13 @@
         <v>13</v>
       </c>
       <c r="B36" s="5">
-        <v>11302</v>
+        <v>8562</v>
       </c>
       <c r="C36" s="5">
-        <v>11588</v>
+        <v>8849</v>
       </c>
       <c r="D36" s="6">
-        <v>211</v>
+        <v>32</v>
       </c>
       <c r="E36" s="5">
         <v>0</v>
@@ -1544,7 +1539,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -1552,16 +1547,16 @@
         <v>13</v>
       </c>
       <c r="B37" s="5">
-        <v>11589</v>
+        <v>11018</v>
       </c>
       <c r="C37" s="5">
-        <v>11830</v>
+        <v>11301</v>
       </c>
       <c r="D37" s="6">
-        <v>147</v>
-      </c>
-      <c r="E37" s="5">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1574,6 +1569,9 @@
       </c>
       <c r="I37" s="5" t="s">
         <v>18</v>
+      </c>
+      <c r="J37" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -1581,13 +1579,13 @@
         <v>13</v>
       </c>
       <c r="B38" s="5">
-        <v>11831</v>
+        <v>11302</v>
       </c>
       <c r="C38" s="5">
-        <v>12118</v>
+        <v>11588</v>
       </c>
       <c r="D38" s="6">
-        <v>125</v>
+        <v>211</v>
       </c>
       <c r="E38" s="5">
         <v>0</v>
@@ -1610,16 +1608,16 @@
         <v>13</v>
       </c>
       <c r="B39" s="5">
-        <v>12119</v>
+        <v>11589</v>
       </c>
       <c r="C39" s="5">
-        <v>12406</v>
+        <v>11830</v>
       </c>
       <c r="D39" s="6">
-        <v>227</v>
+        <v>147</v>
       </c>
       <c r="E39" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1639,13 +1637,13 @@
         <v>13</v>
       </c>
       <c r="B40" s="5">
-        <v>12653</v>
+        <v>11831</v>
       </c>
       <c r="C40" s="5">
-        <v>12940</v>
+        <v>12118</v>
       </c>
       <c r="D40" s="6">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="E40" s="5">
         <v>0</v>
@@ -1665,60 +1663,60 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B41" s="5">
-        <v>1</v>
+        <v>12119</v>
       </c>
       <c r="C41" s="5">
-        <v>135</v>
+        <v>12406</v>
       </c>
       <c r="D41" s="6">
-        <v>138</v>
+        <v>227</v>
       </c>
       <c r="E41" s="5">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B42" s="5">
-        <v>136</v>
+        <v>12653</v>
       </c>
       <c r="C42" s="5">
-        <v>242</v>
-      </c>
-      <c r="D42" s="4">
-        <v>164</v>
+        <v>12940</v>
+      </c>
+      <c r="D42" s="6">
+        <v>153</v>
       </c>
       <c r="E42" s="5">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
@@ -1726,13 +1724,13 @@
         <v>20</v>
       </c>
       <c r="B43" s="5">
-        <v>243</v>
+        <v>1</v>
       </c>
       <c r="C43" s="5">
-        <v>384</v>
+        <v>135</v>
       </c>
       <c r="D43" s="6">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E43" s="5">
         <v>0</v>
@@ -1747,39 +1745,36 @@
         <v>1</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="3">
-        <v>385</v>
-      </c>
-      <c r="C44" s="3">
-        <v>455</v>
+      <c r="B44" s="5">
+        <v>136</v>
+      </c>
+      <c r="C44" s="5">
+        <v>242</v>
       </c>
       <c r="D44" s="4">
-        <v>15</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0</v>
-      </c>
-      <c r="F44" s="3">
-        <v>1</v>
-      </c>
-      <c r="G44" s="3">
-        <v>0</v>
-      </c>
-      <c r="H44" s="3">
-        <v>1</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>27</v>
+        <v>164</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>1</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -1787,13 +1782,13 @@
         <v>20</v>
       </c>
       <c r="B45" s="5">
-        <v>456</v>
+        <v>243</v>
       </c>
       <c r="C45" s="5">
-        <v>561</v>
+        <v>384</v>
       </c>
       <c r="D45" s="6">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="E45" s="5">
         <v>0</v>
@@ -1808,51 +1803,53 @@
         <v>1</v>
       </c>
       <c r="I45" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="3">
+        <v>385</v>
+      </c>
+      <c r="C46" s="3">
+        <v>455</v>
+      </c>
+      <c r="D46" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="5">
-        <v>1601</v>
-      </c>
-      <c r="C46" s="5">
-        <v>1755</v>
-      </c>
-      <c r="D46" s="6">
-        <v>55</v>
-      </c>
-      <c r="E46" s="5">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46" s="5">
-        <v>0</v>
-      </c>
-      <c r="H46" s="5">
-        <v>1</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J46" s="7"/>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B47" s="5">
-        <v>3076</v>
+        <v>456</v>
       </c>
       <c r="C47" s="5">
-        <v>3230</v>
+        <v>561</v>
       </c>
       <c r="D47" s="6">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="E47" s="5">
         <v>0</v>
@@ -1867,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -1875,13 +1872,13 @@
         <v>20</v>
       </c>
       <c r="B48" s="5">
-        <v>3319</v>
+        <v>1601</v>
       </c>
       <c r="C48" s="5">
-        <v>3475</v>
+        <v>1755</v>
       </c>
       <c r="D48" s="6">
-        <v>360</v>
+        <v>55</v>
       </c>
       <c r="E48" s="5">
         <v>0</v>
@@ -1896,21 +1893,22 @@
         <v>1</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B49" s="5">
-        <v>3549</v>
+        <v>3076</v>
       </c>
       <c r="C49" s="5">
-        <v>3701</v>
+        <v>3230</v>
       </c>
       <c r="D49" s="6">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="E49" s="5">
         <v>0</v>
@@ -1925,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -1933,27 +1931,85 @@
         <v>20</v>
       </c>
       <c r="B50" s="5">
+        <v>3319</v>
+      </c>
+      <c r="C50" s="5">
+        <v>3475</v>
+      </c>
+      <c r="D50" s="6">
+        <v>360</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" s="5">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
+        <v>1</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="5">
+        <v>3549</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3701</v>
+      </c>
+      <c r="D51" s="6">
+        <v>105</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" s="5">
+        <v>0</v>
+      </c>
+      <c r="H51" s="5">
+        <v>1</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="5">
         <v>4272</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C52" s="5">
         <v>4423</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D52" s="6">
         <v>283</v>
       </c>
-      <c r="E50" s="5">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" s="5">
-        <v>0</v>
-      </c>
-      <c r="H50" s="5">
-        <v>1</v>
-      </c>
-      <c r="I50" s="5" t="s">
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0</v>
+      </c>
+      <c r="H52" s="5">
+        <v>1</v>
+      </c>
+      <c r="I52" s="5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started to make the codebase "publication ready".
Need to 1. fix the cross validation function b/c I misunderstood what it was 2. add more comments 3. fix EasyGV to read from the right file
</commit_message>
<xml_diff>
--- a/graphics_scripts/data/manual_calculations.xlsx
+++ b/graphics_scripts/data/manual_calculations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merlin\Documents\TAMU\Research - Dr. Gaynanova\iglu\Official MAGE Data Repo\mage_algorithm_data\graphics_scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D847D12-BA9E-4FD4-A585-933C5E9E2C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
     <t>data set</t>
   </si>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -473,19 +474,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="8.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -517,7 +518,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -546,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -575,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -604,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -633,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -662,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -691,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -718,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -747,7 +748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -776,7 +777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -805,7 +806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -834,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -866,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -895,7 +896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -924,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -956,7 +957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
@@ -985,7 +986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -1014,7 +1015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
@@ -1046,152 +1047,167 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="3">
         <v>7697</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>7953</v>
       </c>
       <c r="D20" s="4">
         <v>52</v>
       </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" s="5">
-        <v>1</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5" t="s">
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="J20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="3">
         <v>7954</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>8128</v>
       </c>
       <c r="D21" s="4">
         <v>75</v>
       </c>
-      <c r="E21" s="5">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>1</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5" t="s">
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+      <c r="J21" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="3">
         <v>8129</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>8343</v>
       </c>
       <c r="D22" s="4">
         <v>46</v>
       </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22" s="5">
-        <v>1</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5" t="s">
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="J22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="3">
         <v>8344</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>8513</v>
       </c>
       <c r="D23" s="4">
         <v>40</v>
       </c>
-      <c r="E23" s="5">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5" t="s">
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
+      <c r="J23" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="3">
         <v>8514</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>8745</v>
       </c>
       <c r="D24" s="4">
         <v>61</v>
       </c>
-      <c r="E24" s="5">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0</v>
-      </c>
-      <c r="I24" s="5" t="s">
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J24" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>13</v>
       </c>
@@ -1220,7 +1236,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -1249,7 +1265,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>13</v>
       </c>
@@ -1278,7 +1294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -1307,7 +1323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>13</v>
       </c>
@@ -1336,7 +1352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
@@ -1365,7 +1381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>13</v>
       </c>
@@ -1397,7 +1413,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
@@ -1513,7 +1529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="5" t="s">
         <v>13</v>
       </c>
@@ -1542,7 +1558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>13</v>
       </c>
@@ -1574,7 +1590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
@@ -1603,7 +1619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="5" t="s">
         <v>13</v>
       </c>
@@ -1632,7 +1648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
@@ -1661,7 +1677,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>13</v>
       </c>
@@ -1690,7 +1706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="5" t="s">
         <v>13</v>
       </c>
@@ -1719,7 +1735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
         <v>20</v>
       </c>
@@ -1748,7 +1764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="5" t="s">
         <v>20</v>
       </c>
@@ -1777,7 +1793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="5" t="s">
         <v>20</v>
       </c>
@@ -1806,7 +1822,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>20</v>
       </c>
@@ -1838,7 +1854,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
         <v>20</v>
       </c>
@@ -1867,7 +1883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="5" t="s">
         <v>20</v>
       </c>
@@ -1897,7 +1913,7 @@
       </c>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
         <v>20</v>
       </c>
@@ -1926,7 +1942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="5" t="s">
         <v>20</v>
       </c>
@@ -1955,7 +1971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="5" t="s">
         <v>20</v>
       </c>
@@ -1984,7 +2000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Change data set to dataset
</commit_message>
<xml_diff>
--- a/graphics_scripts/data/manual_calculations.xlsx
+++ b/graphics_scripts/data/manual_calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merlin\Documents\TAMU\Research - Dr. Gaynanova\iglu\Official MAGE Data Repo\mage_algorithm_data\graphics_scripts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Irina/Google Drive/MacLaptop/Research/github/mage_algorithm_data/graphics_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D847D12-BA9E-4FD4-A585-933C5E9E2C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C2B15B-B822-294F-A560-51D88386DCF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
-    <t>data set</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>microscopic gap</t>
+  </si>
+  <si>
+    <t>dataset</t>
   </si>
 </sst>
 </file>
@@ -477,50 +477,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="8.73046875" style="1"/>
+    <col min="4" max="4" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -547,9 +545,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5">
         <v>60</v>
@@ -576,9 +574,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5">
         <v>353</v>
@@ -605,9 +603,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>646</v>
@@ -634,9 +632,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>940</v>
@@ -663,9 +661,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1497</v>
@@ -692,9 +690,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>1788</v>
@@ -719,9 +717,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -745,12 +743,12 @@
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>245</v>
@@ -774,12 +772,12 @@
         <v>0</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5">
         <v>532</v>
@@ -803,12 +801,12 @@
         <v>0</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5">
         <v>755</v>
@@ -832,12 +830,12 @@
         <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5">
         <v>849</v>
@@ -861,15 +859,15 @@
         <v>0</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="5">
         <v>1102</v>
@@ -893,12 +891,12 @@
         <v>0</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="5">
         <v>1380</v>
@@ -922,12 +920,12 @@
         <v>0</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="5">
         <v>1667</v>
@@ -951,15 +949,15 @@
         <v>0</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5">
         <v>1847</v>
@@ -983,12 +981,12 @@
         <v>0</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="5">
         <v>2125</v>
@@ -1012,12 +1010,12 @@
         <v>0</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="5">
         <v>2304</v>
@@ -1041,15 +1039,15 @@
         <v>0</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3">
         <v>7697</v>
@@ -1073,15 +1071,15 @@
         <v>0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="3">
         <v>7954</v>
@@ -1105,15 +1103,15 @@
         <v>0</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3">
         <v>8129</v>
@@ -1137,15 +1135,15 @@
         <v>0</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="3">
         <v>8344</v>
@@ -1169,15 +1167,15 @@
         <v>0</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="3">
         <v>8514</v>
@@ -1201,15 +1199,15 @@
         <v>0</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="5">
         <v>405</v>
@@ -1233,12 +1231,12 @@
         <v>2</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="5">
         <v>2994</v>
@@ -1262,12 +1260,12 @@
         <v>2</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="5">
         <v>3282</v>
@@ -1291,12 +1289,12 @@
         <v>2</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B28" s="5">
         <v>3570</v>
@@ -1320,12 +1318,12 @@
         <v>2</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="5">
         <v>3858</v>
@@ -1349,12 +1347,12 @@
         <v>2</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="5">
         <v>4145</v>
@@ -1378,12 +1376,12 @@
         <v>2</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B31" s="5">
         <v>5746</v>
@@ -1407,15 +1405,15 @@
         <v>2</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="5">
         <v>7413</v>
@@ -1439,12 +1437,12 @@
         <v>2</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="5">
         <v>7699</v>
@@ -1468,12 +1466,12 @@
         <v>2</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" s="5">
         <v>7986</v>
@@ -1497,12 +1495,12 @@
         <v>2</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="5">
         <v>8274</v>
@@ -1526,12 +1524,12 @@
         <v>2</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" s="5">
         <v>8562</v>
@@ -1555,12 +1553,12 @@
         <v>2</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" s="5">
         <v>11018</v>
@@ -1584,15 +1582,15 @@
         <v>2</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="5">
         <v>11302</v>
@@ -1616,12 +1614,12 @@
         <v>2</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B39" s="5">
         <v>11589</v>
@@ -1645,12 +1643,12 @@
         <v>2</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" s="5">
         <v>11831</v>
@@ -1674,12 +1672,12 @@
         <v>2</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B41" s="5">
         <v>12119</v>
@@ -1703,12 +1701,12 @@
         <v>2</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" s="5">
         <v>12653</v>
@@ -1732,12 +1730,12 @@
         <v>2</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -1761,12 +1759,12 @@
         <v>1</v>
       </c>
       <c r="I43" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A44" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B44" s="5">
         <v>136</v>
@@ -1790,12 +1788,12 @@
         <v>1</v>
       </c>
       <c r="I44" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A45" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B45" s="5">
         <v>243</v>
@@ -1819,12 +1817,12 @@
         <v>1</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" s="3">
         <v>385</v>
@@ -1848,15 +1846,15 @@
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="5">
         <v>456</v>
@@ -1880,12 +1878,12 @@
         <v>1</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="5">
         <v>1601</v>
@@ -1909,13 +1907,13 @@
         <v>1</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B49" s="5">
         <v>3076</v>
@@ -1939,12 +1937,12 @@
         <v>1</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="5">
         <v>3319</v>
@@ -1968,12 +1966,12 @@
         <v>1</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B51" s="5">
         <v>3549</v>
@@ -1997,12 +1995,12 @@
         <v>1</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52" s="5">
         <v>4272</v>
@@ -2026,7 +2024,7 @@
         <v>1</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>